<commit_message>
Aprobacion de cambios Julian Aguilar
</commit_message>
<xml_diff>
--- a/Documentación/Errores.xlsx
+++ b/Documentación/Errores.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnsdirm\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>No Error</t>
   </si>
@@ -66,6 +61,9 @@
   </si>
   <si>
     <t>no hay relacion con proveedores y materia prima</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -163,7 +161,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -198,7 +196,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,7 +373,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -386,7 +384,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,6 +414,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -424,6 +425,9 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -432,6 +436,9 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -440,6 +447,9 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -448,6 +458,9 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -456,6 +469,9 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -464,6 +480,9 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -472,6 +491,9 @@
       <c r="B9" t="s">
         <v>11</v>
       </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -480,6 +502,9 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -487,6 +512,9 @@
       </c>
       <c r="B11" t="s">
         <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>